<commit_message>
Added all measurements and made Polar diagram
	modified:   exp4/data/Airfoil.xlsx
</commit_message>
<xml_diff>
--- a/exp4/data/Airfoil.xlsx
+++ b/exp4/data/Airfoil.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="198" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="117" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
   <si>
     <t>p (mmWs)</t>
   </si>
@@ -24,6 +24,87 @@
   </si>
   <si>
     <t>y (mm)</t>
+  </si>
+  <si>
+    <t>Airspeed:</t>
+  </si>
+  <si>
+    <t>[m/s]</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Stdev</t>
+  </si>
+  <si>
+    <t>StdErrMean</t>
+  </si>
+  <si>
+    <t>Resistance</t>
+  </si>
+  <si>
+    <t>vertical</t>
+  </si>
+  <si>
+    <t>[g]</t>
+  </si>
+  <si>
+    <t>-20°</t>
+  </si>
+  <si>
+    <t>-15°</t>
+  </si>
+  <si>
+    <t>-10°</t>
+  </si>
+  <si>
+    <t>-5°</t>
+  </si>
+  <si>
+    <t>0°</t>
+  </si>
+  <si>
+    <t>5°</t>
+  </si>
+  <si>
+    <t>10°</t>
+  </si>
+  <si>
+    <t>15°</t>
+  </si>
+  <si>
+    <t>20°</t>
+  </si>
+  <si>
+    <t>StErrMean</t>
+  </si>
+  <si>
+    <t>Lift</t>
+  </si>
+  <si>
+    <t>horizontal</t>
+  </si>
+  <si>
+    <t>Wind</t>
+  </si>
+  <si>
+    <t>14.5 m/s</t>
+  </si>
+  <si>
+    <t>Polar Diagram</t>
+  </si>
+  <si>
+    <t>Angle </t>
+  </si>
+  <si>
+    <t>F_res</t>
+  </si>
+  <si>
+    <t>F_lift</t>
+  </si>
+  <si>
+    <t>ca/cw</t>
   </si>
 </sst>
 </file>
@@ -33,9 +114,10 @@
   <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="8">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -54,13 +136,71 @@
       <family val="0"/>
       <sz val="10"/>
     </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <b val="true"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <sz val="13"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <sz val="9"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF47B8B8"/>
+        <bgColor rgb="FF33A3A3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF33A3A3"/>
+        <bgColor rgb="FF47B8B8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF94BD5E"/>
+        <bgColor rgb="FF7DA647"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7DA647"/>
+        <bgColor rgb="FF94BD5E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEB613D"/>
+        <bgColor rgb="FFFF8080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB84747"/>
+        <bgColor rgb="FF993366"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -97,8 +237,52 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="12">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="5" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="5" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="6" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="6" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="7" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -130,7 +314,7 @@
       <rgbColor rgb="FFB3B3B3"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFB84747"/>
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
@@ -154,15 +338,15 @@
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FF47B8B8"/>
+      <rgbColor rgb="FF94BD5E"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFEB613D"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF7DA647"/>
       <rgbColor rgb="FF004586"/>
-      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF33A3A3"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
@@ -174,7 +358,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -187,7 +371,7 @@
           <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="004586"/>
+              <a:srgbClr val="99ccff"/>
             </a:solidFill>
           </c:spPr>
           <c:marker/>
@@ -288,11 +472,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="39462397"/>
-        <c:axId val="26090566"/>
+        <c:axId val="87838211"/>
+        <c:axId val="73387788"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="39462397"/>
+        <c:axId val="87838211"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-10"/>
@@ -301,8 +485,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="26090566"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="73387788"/>
+        <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
             <a:solidFill>
@@ -312,7 +496,7 @@
         </c:spPr>
       </c:valAx>
       <c:valAx>
-        <c:axId val="26090566"/>
+        <c:axId val="73387788"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -329,7 +513,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39462397"/>
+        <c:crossAx val="87838211"/>
         <c:crossesAt val="0"/>
         <c:majorUnit val="10"/>
         <c:spPr>
@@ -362,20 +546,274 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr sz="1300"/>
+              <a:t>Polar Diagram</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$55:$J$55</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>-20°</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-15°</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-10°</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-5°</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0°</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5°</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10°</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15°</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20°</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$56:$J$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.21582</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.161865</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.12753</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.11772</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.11772</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.13734</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.15696</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.1962</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.24525</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$57:$J$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.03924</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0981</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.161865</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.22563</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2943</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.36297</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.41202</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.51012</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.42183</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="30689191"/>
+        <c:axId val="98668157"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="30689191"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:title>
+          <c:layout/>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr sz="900"/>
+                  <a:t>F_r</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+        </c:title>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="98668157"/>
+        <c:crosses val="autoZero"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="98668157"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:title>
+          <c:layout/>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr sz="900"/>
+                  <a:t>F_l</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+        </c:title>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="30689191"/>
+        <c:crosses val="autoZero"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+      </c:valAx>
+      <c:spPr>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>733320</xdr:colOff>
+      <xdr:colOff>760320</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>105480</xdr:rowOff>
+      <xdr:rowOff>96840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>713520</xdr:colOff>
+      <xdr:colOff>740160</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>21960</xdr:rowOff>
+      <xdr:rowOff>12600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -383,12 +821,42 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3984480" y="267840"/>
-        <a:ext cx="7295400" cy="3375360"/>
+        <a:off x="4011480" y="259200"/>
+        <a:ext cx="7295040" cy="3374640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>332640</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>151560</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>352440</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>121680</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="1" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="10899000" y="4748040"/>
+        <a:ext cx="7335000" cy="5000760"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -402,10 +870,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B3:D16"/>
+  <dimension ref="A3:M58"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B21" activeCellId="0" pane="topLeft" sqref="B21"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A10" view="normal" windowProtection="false" workbookViewId="0" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100">
+      <selection activeCell="L55" activeCellId="0" pane="topLeft" sqref="L55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -413,7 +881,7 @@
     <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="3">
       <c r="B3" s="0" t="s">
         <v>0</v>
       </c>
@@ -424,7 +892,10 @@
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="4">
+      <c r="A4" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="B4" s="0" t="n">
         <v>-0.1</v>
       </c>
@@ -435,7 +906,10 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="5">
+      <c r="A5" s="0" t="n">
+        <v>13</v>
+      </c>
       <c r="B5" s="0" t="n">
         <v>1.5</v>
       </c>
@@ -446,7 +920,10 @@
         <v>-1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="6">
+      <c r="A6" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="B6" s="0" t="n">
         <v>-1</v>
       </c>
@@ -457,7 +934,10 @@
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="7">
+      <c r="A7" s="0" t="n">
+        <v>12</v>
+      </c>
       <c r="B7" s="0" t="n">
         <v>2.25</v>
       </c>
@@ -468,7 +948,10 @@
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="8">
+      <c r="A8" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="B8" s="0" t="n">
         <v>-5.6</v>
       </c>
@@ -479,7 +962,10 @@
         <v>29</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="9">
+      <c r="A9" s="0" t="n">
+        <v>11</v>
+      </c>
       <c r="B9" s="0" t="n">
         <v>-0.8</v>
       </c>
@@ -490,7 +976,10 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="10">
+      <c r="A10" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="B10" s="0" t="n">
         <v>-14.6</v>
       </c>
@@ -501,7 +990,10 @@
         <v>33</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
       <c r="B11" s="0" t="n">
         <v>-7.5</v>
       </c>
@@ -512,7 +1004,10 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="12">
+      <c r="A12" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="B12" s="0" t="n">
         <v>-12.85</v>
       </c>
@@ -523,7 +1018,10 @@
         <v>31</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="13">
+      <c r="A13" s="0" t="n">
+        <v>9</v>
+      </c>
       <c r="B13" s="0" t="n">
         <v>-8.8</v>
       </c>
@@ -534,7 +1032,10 @@
         <v>4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="14">
+      <c r="A14" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="B14" s="0" t="n">
         <v>0.5</v>
       </c>
@@ -545,7 +1046,10 @@
         <v>25</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="15">
+      <c r="A15" s="0" t="n">
+        <v>8</v>
+      </c>
       <c r="B15" s="0" t="n">
         <v>5.4</v>
       </c>
@@ -556,7 +1060,10 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="16">
+      <c r="A16" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="B16" s="0" t="n">
         <v>15.5</v>
       </c>
@@ -565,6 +1072,671 @@
       </c>
       <c r="D16" s="0" t="n">
         <v>16</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="26">
+      <c r="B26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="J26" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="27">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="D27" s="2" t="n">
+        <v>14.7</v>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>14.6</v>
+      </c>
+      <c r="F27" s="2" t="n">
+        <v>14.8</v>
+      </c>
+      <c r="G27" s="2" t="n">
+        <v>14.7</v>
+      </c>
+      <c r="H27" s="2" t="n">
+        <v>14.75</v>
+      </c>
+      <c r="J27" s="3" t="n">
+        <f aca="false">AVERAGE(C27:G27)</f>
+        <v>14.76</v>
+      </c>
+      <c r="K27" s="3" t="n">
+        <f aca="false">STDEV(C27:H27)</f>
+        <v>0.135708019905482</v>
+      </c>
+      <c r="L27" s="3" t="n">
+        <f aca="false">K27/SQRT(COUNT(C27:H27))</f>
+        <v>0.055402567128649</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="30">
+      <c r="B30" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K30" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L30" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M30" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="31">
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5" t="n">
+        <v>22</v>
+      </c>
+      <c r="F31" s="5" t="n">
+        <v>16.5</v>
+      </c>
+      <c r="G31" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="H31" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="I31" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="J31" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="K31" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="L31" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="M31" s="5" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="32">
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5" t="n">
+        <v>22</v>
+      </c>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5" t="n">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="33">
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5" t="n">
+        <v>22</v>
+      </c>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="35">
+      <c r="C35" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6" t="n">
+        <f aca="false">AVERAGE(E31:E33)</f>
+        <v>22</v>
+      </c>
+      <c r="F35" s="6" t="n">
+        <f aca="false">AVERAGE(F31:F33)</f>
+        <v>16.5</v>
+      </c>
+      <c r="G35" s="6" t="n">
+        <f aca="false">AVERAGE(G31:G33)</f>
+        <v>13</v>
+      </c>
+      <c r="H35" s="6" t="n">
+        <f aca="false">AVERAGE(H31:H33)</f>
+        <v>12</v>
+      </c>
+      <c r="I35" s="6" t="n">
+        <f aca="false">AVERAGE(I31:I33)</f>
+        <v>12</v>
+      </c>
+      <c r="J35" s="6" t="n">
+        <f aca="false">AVERAGE(J31:J33)</f>
+        <v>14</v>
+      </c>
+      <c r="K35" s="6" t="n">
+        <f aca="false">AVERAGE(K31:K33)</f>
+        <v>16</v>
+      </c>
+      <c r="L35" s="6" t="n">
+        <f aca="false">AVERAGE(L31:L33)</f>
+        <v>20</v>
+      </c>
+      <c r="M35" s="6" t="n">
+        <f aca="false">AVERAGE(M31:M33)</f>
+        <v>24.75</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="36">
+      <c r="C36" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6" t="n">
+        <f aca="false">STDEV(E31:E34)</f>
+        <v>0</v>
+      </c>
+      <c r="F36" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I36" s="6" t="n">
+        <f aca="false">STDEV(I31:I34)</f>
+        <v>0</v>
+      </c>
+      <c r="J36" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K36" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L36" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M36" s="7" t="n">
+        <f aca="false">STDEV(M31:M33)</f>
+        <v>0.353553390593274</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="37">
+      <c r="C37" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6" t="n">
+        <f aca="false">E36/SQRT(COUNT(E31:E33))</f>
+        <v>0</v>
+      </c>
+      <c r="F37" s="6" t="n">
+        <f aca="false">F36/SQRT(COUNT(F31:F33))</f>
+        <v>0</v>
+      </c>
+      <c r="G37" s="6" t="n">
+        <f aca="false">G36/SQRT(COUNT(G31:G33))</f>
+        <v>0</v>
+      </c>
+      <c r="H37" s="6" t="n">
+        <f aca="false">H36/SQRT(COUNT(H31:H33))</f>
+        <v>0</v>
+      </c>
+      <c r="I37" s="6" t="n">
+        <f aca="false">I36/SQRT(COUNT(I31:I33))</f>
+        <v>0</v>
+      </c>
+      <c r="J37" s="6" t="n">
+        <f aca="false">J36/SQRT(COUNT(J31:J33))</f>
+        <v>0</v>
+      </c>
+      <c r="K37" s="6" t="n">
+        <f aca="false">K36/SQRT(COUNT(K31:K33))</f>
+        <v>0</v>
+      </c>
+      <c r="L37" s="6" t="n">
+        <f aca="false">L36/SQRT(COUNT(L31:L33))</f>
+        <v>0</v>
+      </c>
+      <c r="M37" s="6" t="n">
+        <f aca="false">M36/SQRT(COUNT(M31:M33))</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="40">
+      <c r="B40" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H40" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I40" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J40" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K40" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L40" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="M40" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="41">
+      <c r="B41" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="F41" s="9" t="n">
+        <v>10</v>
+      </c>
+      <c r="G41" s="9" t="n">
+        <v>16.5</v>
+      </c>
+      <c r="H41" s="9" t="n">
+        <v>23</v>
+      </c>
+      <c r="I41" s="9" t="n">
+        <v>30</v>
+      </c>
+      <c r="J41" s="9" t="n">
+        <v>37</v>
+      </c>
+      <c r="K41" s="9" t="n">
+        <v>42</v>
+      </c>
+      <c r="L41" s="9" t="n">
+        <v>52</v>
+      </c>
+      <c r="M41" s="9" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="42">
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="9" t="n">
+        <v>35</v>
+      </c>
+      <c r="K42" s="9"/>
+      <c r="L42" s="9"/>
+      <c r="M42" s="9"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="43">
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="9"/>
+      <c r="J43" s="9" t="n">
+        <v>36</v>
+      </c>
+      <c r="K43" s="9"/>
+      <c r="L43" s="9"/>
+      <c r="M43" s="9"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="45">
+      <c r="C45" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10" t="n">
+        <f aca="false">AVERAGE(E41:E43)</f>
+        <v>4</v>
+      </c>
+      <c r="F45" s="10" t="n">
+        <f aca="false">AVERAGE(F41:F43)</f>
+        <v>10</v>
+      </c>
+      <c r="G45" s="10" t="n">
+        <f aca="false">AVERAGE(G41:G43)</f>
+        <v>16.5</v>
+      </c>
+      <c r="H45" s="10" t="n">
+        <f aca="false">AVERAGE(H41:H43)</f>
+        <v>23</v>
+      </c>
+      <c r="I45" s="10" t="n">
+        <f aca="false">AVERAGE(I41:I43)</f>
+        <v>30</v>
+      </c>
+      <c r="J45" s="10" t="n">
+        <f aca="false">AVERAGE(J41:J43)</f>
+        <v>36</v>
+      </c>
+      <c r="K45" s="10" t="n">
+        <f aca="false">AVERAGE(K41:K43)</f>
+        <v>42</v>
+      </c>
+      <c r="L45" s="10" t="n">
+        <f aca="false">AVERAGE(L41:L43)</f>
+        <v>52</v>
+      </c>
+      <c r="M45" s="10" t="n">
+        <f aca="false">AVERAGE(M41:M43)</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="46">
+      <c r="C46" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H46" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I46" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J46" s="10" t="n">
+        <f aca="false">STDEV(J41:J43)</f>
+        <v>1</v>
+      </c>
+      <c r="K46" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L46" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M46" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="47">
+      <c r="C47" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10" t="n">
+        <f aca="false">E46/SQRT(COUNT(E41:E43))</f>
+        <v>0</v>
+      </c>
+      <c r="F47" s="10" t="n">
+        <f aca="false">F46/SQRT(COUNT(F41:F43))</f>
+        <v>0</v>
+      </c>
+      <c r="G47" s="10" t="n">
+        <f aca="false">G46/SQRT(COUNT(G41:G43))</f>
+        <v>0</v>
+      </c>
+      <c r="H47" s="10" t="n">
+        <f aca="false">H46/SQRT(COUNT(H41:H43))</f>
+        <v>0</v>
+      </c>
+      <c r="I47" s="10" t="n">
+        <f aca="false">I46/SQRT(COUNT(I41:I43))</f>
+        <v>0</v>
+      </c>
+      <c r="J47" s="10" t="n">
+        <f aca="false">J46/SQRT(COUNT(J41:J43))</f>
+        <v>0.577350269189626</v>
+      </c>
+      <c r="K47" s="10" t="n">
+        <f aca="false">K46/SQRT(COUNT(K41:K43))</f>
+        <v>0</v>
+      </c>
+      <c r="L47" s="10" t="n">
+        <f aca="false">L46/SQRT(COUNT(L41:L43))</f>
+        <v>0</v>
+      </c>
+      <c r="M47" s="10" t="n">
+        <f aca="false">M46/SQRT(COUNT(M41:M43))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="53">
+      <c r="B53" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="55">
+      <c r="A55" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F55" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G55" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H55" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I55" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J55" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="56">
+      <c r="A56" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B56" s="0" t="n">
+        <f aca="false">E31*9.81/1000</f>
+        <v>0.21582</v>
+      </c>
+      <c r="C56" s="0" t="n">
+        <f aca="false">F31*9.81/1000</f>
+        <v>0.161865</v>
+      </c>
+      <c r="D56" s="0" t="n">
+        <f aca="false">G31*9.81/1000</f>
+        <v>0.12753</v>
+      </c>
+      <c r="E56" s="0" t="n">
+        <f aca="false">H31*9.81/1000</f>
+        <v>0.11772</v>
+      </c>
+      <c r="F56" s="0" t="n">
+        <f aca="false">I31*9.81/1000</f>
+        <v>0.11772</v>
+      </c>
+      <c r="G56" s="0" t="n">
+        <f aca="false">J31*9.81/1000</f>
+        <v>0.13734</v>
+      </c>
+      <c r="H56" s="0" t="n">
+        <f aca="false">K31*9.81/1000</f>
+        <v>0.15696</v>
+      </c>
+      <c r="I56" s="0" t="n">
+        <f aca="false">L31*9.81/1000</f>
+        <v>0.1962</v>
+      </c>
+      <c r="J56" s="0" t="n">
+        <f aca="false">M31*9.81/1000</f>
+        <v>0.24525</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="57">
+      <c r="A57" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <f aca="false">E41*9.81/1000</f>
+        <v>0.03924</v>
+      </c>
+      <c r="C57" s="0" t="n">
+        <f aca="false">F41*9.81/1000</f>
+        <v>0.0981</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <f aca="false">G41*9.81/1000</f>
+        <v>0.161865</v>
+      </c>
+      <c r="E57" s="0" t="n">
+        <f aca="false">H41*9.81/1000</f>
+        <v>0.22563</v>
+      </c>
+      <c r="F57" s="0" t="n">
+        <f aca="false">I41*9.81/1000</f>
+        <v>0.2943</v>
+      </c>
+      <c r="G57" s="0" t="n">
+        <f aca="false">J41*9.81/1000</f>
+        <v>0.36297</v>
+      </c>
+      <c r="H57" s="0" t="n">
+        <f aca="false">K41*9.81/1000</f>
+        <v>0.41202</v>
+      </c>
+      <c r="I57" s="0" t="n">
+        <f aca="false">L41*9.81/1000</f>
+        <v>0.51012</v>
+      </c>
+      <c r="J57" s="0" t="n">
+        <f aca="false">M41*9.81/1000</f>
+        <v>0.42183</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="58">
+      <c r="A58" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B58" s="0" t="n">
+        <f aca="false">B57/B56</f>
+        <v>0.181818181818182</v>
+      </c>
+      <c r="C58" s="0" t="n">
+        <f aca="false">C57/C56</f>
+        <v>0.606060606060606</v>
+      </c>
+      <c r="D58" s="0" t="n">
+        <f aca="false">D57/D56</f>
+        <v>1.26923076923077</v>
+      </c>
+      <c r="E58" s="0" t="n">
+        <f aca="false">E57/E56</f>
+        <v>1.91666666666667</v>
+      </c>
+      <c r="F58" s="0" t="n">
+        <f aca="false">F57/F56</f>
+        <v>2.5</v>
+      </c>
+      <c r="G58" s="0" t="n">
+        <f aca="false">G57/G56</f>
+        <v>2.64285714285714</v>
+      </c>
+      <c r="H58" s="0" t="n">
+        <f aca="false">H57/H56</f>
+        <v>2.625</v>
+      </c>
+      <c r="I58" s="0" t="n">
+        <f aca="false">I57/I56</f>
+        <v>2.6</v>
+      </c>
+      <c r="J58" s="0" t="n">
+        <f aca="false">J57/J56</f>
+        <v>1.72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Quite some advancements to the report
	modified:   data/Airfoil.xlsx
	modified:   report/diag/integral.nb
	new file:   report/diag/polar_diag.pdf
	new file:   report/diag/pressure_points.pdf
	modified:   report/diag/wing_profile.nb
	new file:   report/diag/wing_profile.pdf
	modified:   report/report4.tex
</commit_message>
<xml_diff>
--- a/exp4/data/Airfoil.xlsx
+++ b/exp4/data/Airfoil.xlsx
@@ -95,7 +95,7 @@
     <t>Polar Diagram</t>
   </si>
   <si>
-    <t>Angle </t>
+    <t>Angle</t>
   </si>
   <si>
     <t>F_res</t>
@@ -151,12 +151,12 @@
     <font>
       <name val="Arial"/>
       <family val="2"/>
-      <sz val="13"/>
+      <sz val="20"/>
     </font>
     <font>
       <name val="Arial"/>
       <family val="2"/>
-      <sz val="9"/>
+      <sz val="14"/>
     </font>
   </fonts>
   <fills count="8">
@@ -237,7 +237,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -263,10 +263,6 @@
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="5" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="5" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -472,11 +468,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="87838211"/>
-        <c:axId val="73387788"/>
+        <c:axId val="82525237"/>
+        <c:axId val="10138935"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87838211"/>
+        <c:axId val="82525237"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-10"/>
@@ -485,7 +481,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73387788"/>
+        <c:crossAx val="10138935"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
@@ -496,7 +492,7 @@
         </c:spPr>
       </c:valAx>
       <c:valAx>
-        <c:axId val="73387788"/>
+        <c:axId val="10138935"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -513,7 +509,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87838211"/>
+        <c:crossAx val="82525237"/>
         <c:crossesAt val="0"/>
         <c:majorUnit val="10"/>
         <c:spPr>
@@ -561,7 +557,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300"/>
+              <a:rPr sz="2000"/>
               <a:t>Polar Diagram</a:t>
             </a:r>
           </a:p>
@@ -695,14 +691,14 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="30689191"/>
-        <c:axId val="98668157"/>
+        <c:axId val="10873303"/>
+        <c:axId val="39911496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="30689191"/>
+        <c:axId val="10873303"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="0"/>
+          <c:min val="-0.05"/>
         </c:scaling>
         <c:title>
           <c:layout/>
@@ -715,18 +711,27 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900"/>
-                  <a:t>F_r</a:t>
+                  <a:rPr sz="1400"/>
+                  <a:t>Fr [N]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
         </c:title>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98668157"/>
+        <c:crossAx val="39911496"/>
         <c:crosses val="autoZero"/>
         <c:spPr>
           <a:ln>
@@ -737,7 +742,7 @@
         </c:spPr>
       </c:valAx>
       <c:valAx>
-        <c:axId val="98668157"/>
+        <c:axId val="39911496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -752,8 +757,8 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900"/>
-                  <a:t>F_l</a:t>
+                  <a:rPr sz="1400"/>
+                  <a:t>Fl [N]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -772,8 +777,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="30689191"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="10873303"/>
+        <c:crosses val="min"/>
         <c:spPr>
           <a:ln>
             <a:solidFill>
@@ -805,15 +810,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>760320</xdr:colOff>
+      <xdr:colOff>787320</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>96840</xdr:rowOff>
+      <xdr:rowOff>87840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>740160</xdr:colOff>
+      <xdr:colOff>766800</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>12600</xdr:rowOff>
+      <xdr:rowOff>3240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -821,8 +826,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4011480" y="259200"/>
-        <a:ext cx="7295040" cy="3374640"/>
+        <a:off x="4038480" y="250200"/>
+        <a:ext cx="7294680" cy="3374280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -835,15 +840,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>332640</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>151560</xdr:rowOff>
+      <xdr:colOff>39600</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>73440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>352440</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>121680</xdr:rowOff>
+      <xdr:colOff>655920</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>127440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -851,8 +856,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10899000" y="4748040"/>
-        <a:ext cx="7335000" cy="5000760"/>
+        <a:off x="10605960" y="8083800"/>
+        <a:ext cx="7931520" cy="5572080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -872,8 +877,8 @@
   </sheetPr>
   <dimension ref="A3:M58"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A10" view="normal" windowProtection="false" workbookViewId="0" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100">
-      <selection activeCell="L55" activeCellId="0" pane="topLeft" sqref="L55"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="G43" view="normal" windowProtection="false" workbookViewId="0" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100">
+      <selection activeCell="X86" activeCellId="0" pane="topLeft" sqref="X86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1308,7 +1313,7 @@
       <c r="L36" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="M36" s="7" t="n">
+      <c r="M36" s="6" t="n">
         <f aca="false">STDEV(M31:M33)</f>
         <v>0.353553390593274</v>
       </c>
@@ -1356,231 +1361,231 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="40">
-      <c r="B40" s="8" t="s">
+      <c r="B40" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C40" s="9" t="s">
+      <c r="C40" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D40" s="9" t="s">
+      <c r="D40" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E40" s="9" t="s">
+      <c r="E40" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F40" s="9" t="s">
+      <c r="F40" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G40" s="9" t="s">
+      <c r="G40" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H40" s="9" t="s">
+      <c r="H40" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I40" s="9" t="s">
+      <c r="I40" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="J40" s="9" t="s">
+      <c r="J40" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K40" s="9" t="s">
+      <c r="K40" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="L40" s="9" t="s">
+      <c r="L40" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="M40" s="9" t="s">
+      <c r="M40" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="41">
-      <c r="B41" s="9" t="s">
+      <c r="B41" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C41" s="9" t="s">
+      <c r="C41" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9" t="n">
+      <c r="D41" s="8"/>
+      <c r="E41" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="F41" s="9" t="n">
+      <c r="F41" s="8" t="n">
         <v>10</v>
       </c>
-      <c r="G41" s="9" t="n">
+      <c r="G41" s="8" t="n">
         <v>16.5</v>
       </c>
-      <c r="H41" s="9" t="n">
+      <c r="H41" s="8" t="n">
         <v>23</v>
       </c>
-      <c r="I41" s="9" t="n">
+      <c r="I41" s="8" t="n">
         <v>30</v>
       </c>
-      <c r="J41" s="9" t="n">
+      <c r="J41" s="8" t="n">
         <v>37</v>
       </c>
-      <c r="K41" s="9" t="n">
+      <c r="K41" s="8" t="n">
         <v>42</v>
       </c>
-      <c r="L41" s="9" t="n">
+      <c r="L41" s="8" t="n">
         <v>52</v>
       </c>
-      <c r="M41" s="9" t="n">
+      <c r="M41" s="8" t="n">
         <v>43</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="42">
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
-      <c r="H42" s="9"/>
-      <c r="I42" s="9"/>
-      <c r="J42" s="9" t="n">
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8" t="n">
         <v>35</v>
       </c>
-      <c r="K42" s="9"/>
-      <c r="L42" s="9"/>
-      <c r="M42" s="9"/>
+      <c r="K42" s="8"/>
+      <c r="L42" s="8"/>
+      <c r="M42" s="8"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="43">
-      <c r="B43" s="9"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
-      <c r="I43" s="9"/>
-      <c r="J43" s="9" t="n">
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8" t="n">
         <v>36</v>
       </c>
-      <c r="K43" s="9"/>
-      <c r="L43" s="9"/>
-      <c r="M43" s="9"/>
+      <c r="K43" s="8"/>
+      <c r="L43" s="8"/>
+      <c r="M43" s="8"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="45">
-      <c r="C45" s="10" t="s">
+      <c r="C45" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D45" s="10"/>
-      <c r="E45" s="10" t="n">
+      <c r="D45" s="9"/>
+      <c r="E45" s="9" t="n">
         <f aca="false">AVERAGE(E41:E43)</f>
         <v>4</v>
       </c>
-      <c r="F45" s="10" t="n">
+      <c r="F45" s="9" t="n">
         <f aca="false">AVERAGE(F41:F43)</f>
         <v>10</v>
       </c>
-      <c r="G45" s="10" t="n">
+      <c r="G45" s="9" t="n">
         <f aca="false">AVERAGE(G41:G43)</f>
         <v>16.5</v>
       </c>
-      <c r="H45" s="10" t="n">
+      <c r="H45" s="9" t="n">
         <f aca="false">AVERAGE(H41:H43)</f>
         <v>23</v>
       </c>
-      <c r="I45" s="10" t="n">
+      <c r="I45" s="9" t="n">
         <f aca="false">AVERAGE(I41:I43)</f>
         <v>30</v>
       </c>
-      <c r="J45" s="10" t="n">
+      <c r="J45" s="9" t="n">
         <f aca="false">AVERAGE(J41:J43)</f>
         <v>36</v>
       </c>
-      <c r="K45" s="10" t="n">
+      <c r="K45" s="9" t="n">
         <f aca="false">AVERAGE(K41:K43)</f>
         <v>42</v>
       </c>
-      <c r="L45" s="10" t="n">
+      <c r="L45" s="9" t="n">
         <f aca="false">AVERAGE(L41:L43)</f>
         <v>52</v>
       </c>
-      <c r="M45" s="10" t="n">
+      <c r="M45" s="9" t="n">
         <f aca="false">AVERAGE(M41:M43)</f>
         <v>43</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="46">
-      <c r="C46" s="10" t="s">
+      <c r="C46" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D46" s="10"/>
-      <c r="E46" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F46" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G46" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H46" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="I46" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J46" s="10" t="n">
+      <c r="D46" s="9"/>
+      <c r="E46" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H46" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I46" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J46" s="9" t="n">
         <f aca="false">STDEV(J41:J43)</f>
         <v>1</v>
       </c>
-      <c r="K46" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="L46" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="M46" s="10" t="n">
+      <c r="K46" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L46" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M46" s="9" t="n">
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="47">
-      <c r="C47" s="10" t="s">
+      <c r="C47" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D47" s="10"/>
-      <c r="E47" s="10" t="n">
+      <c r="D47" s="9"/>
+      <c r="E47" s="9" t="n">
         <f aca="false">E46/SQRT(COUNT(E41:E43))</f>
         <v>0</v>
       </c>
-      <c r="F47" s="10" t="n">
+      <c r="F47" s="9" t="n">
         <f aca="false">F46/SQRT(COUNT(F41:F43))</f>
         <v>0</v>
       </c>
-      <c r="G47" s="10" t="n">
+      <c r="G47" s="9" t="n">
         <f aca="false">G46/SQRT(COUNT(G41:G43))</f>
         <v>0</v>
       </c>
-      <c r="H47" s="10" t="n">
+      <c r="H47" s="9" t="n">
         <f aca="false">H46/SQRT(COUNT(H41:H43))</f>
         <v>0</v>
       </c>
-      <c r="I47" s="10" t="n">
+      <c r="I47" s="9" t="n">
         <f aca="false">I46/SQRT(COUNT(I41:I43))</f>
         <v>0</v>
       </c>
-      <c r="J47" s="10" t="n">
+      <c r="J47" s="9" t="n">
         <f aca="false">J46/SQRT(COUNT(J41:J43))</f>
         <v>0.577350269189626</v>
       </c>
-      <c r="K47" s="10" t="n">
+      <c r="K47" s="9" t="n">
         <f aca="false">K46/SQRT(COUNT(K41:K43))</f>
         <v>0</v>
       </c>
-      <c r="L47" s="10" t="n">
+      <c r="L47" s="9" t="n">
         <f aca="false">L46/SQRT(COUNT(L41:L43))</f>
         <v>0</v>
       </c>
-      <c r="M47" s="10" t="n">
+      <c r="M47" s="9" t="n">
         <f aca="false">M46/SQRT(COUNT(M41:M43))</f>
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="53">
-      <c r="B53" s="11" t="s">
+      <c r="B53" s="10" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1616,7 +1621,7 @@
         <v>19</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="56">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="56">
       <c r="A56" s="0" t="s">
         <v>27</v>
       </c>
@@ -1741,11 +1746,11 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="landscape" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader/>
+    <oddFooter/>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>